<commit_message>
perbaikan kelola akun dan ambil data
</commit_message>
<xml_diff>
--- a/public/format_import/tunggakan.xlsx
+++ b/public/format_import/tunggakan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\College\File Kuliah\Tingkat 4\semester 7\Magang\file testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\smart_dashboard_madiun\public\format_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B632091-6B4E-41A1-A425-A2D02F607C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA55FDD-0BDE-46C4-9C13-7F5137208F71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A6EFF871-6199-4902-BB1B-D1DDD94CD454}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" xr2:uid="{A6EFF871-6199-4902-BB1B-D1DDD94CD454}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,24 +33,9 @@
     <t>TAHUN_SPPT</t>
   </si>
   <si>
-    <t>NOMINAL_BAKU</t>
-  </si>
-  <si>
-    <t>NOMINAL_POKOK</t>
-  </si>
-  <si>
     <t>NOMINAL_DENDA</t>
   </si>
   <si>
-    <t>NOMINAL_TERIMA</t>
-  </si>
-  <si>
-    <t>NOP_BAKU</t>
-  </si>
-  <si>
-    <t>NOP_BAYAR</t>
-  </si>
-  <si>
     <t>KECAMATAN</t>
   </si>
   <si>
@@ -61,6 +46,21 @@
   </si>
   <si>
     <t>TANGGAL_UPDATE</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>NOMINAL_TUNGGAKAN</t>
+  </si>
+  <si>
+    <t>NAMA_REKENING</t>
+  </si>
+  <si>
+    <t>PBB_TERUTANG</t>
+  </si>
+  <si>
+    <t>TAHUN_PAJAK</t>
   </si>
 </sst>
 </file>
@@ -99,9 +99,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,61 +424,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14D2812-398C-490B-A63C-1A23B237957E}">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>